<commit_message>
Nab 458 samples project management ja (#96)
* ・「ユーザ」「マネージャ」「メンバ」の表記ゆれを調整
・開始日≧終了日時のエラーメッセージ登録漏れ対応

* プロジェクト更新画面からの「戻る」遷移漏れ対応

* ・「ユーザ」「マネージャ」「メンバ」の表記ゆれを調整
・項目名、項目ID、ドメイン名をテーブル定義、ドメイン定義に合わせて修正

* インデント間違いを修正

* 二重サブミットエラーメッセージの定義漏れ対応

* 誤った修正を戻す対応

* ・文書表現の改善
・誤字修正
・不要な埋め込み文字定義を削除

* 不要な空行を削除

* 二重サブミットエラーメッセージの定義漏れ対応
</commit_message>
<xml_diff>
--- a/サンプルプロジェクト/設計書/A1_プロジェクト管理システム/010_要件定義/040_画面設計/画面遷移図_A1_プロジェクト管理システム.xlsx
+++ b/サンプルプロジェクト/設計書/A1_プロジェクト管理システム/010_要件定義/040_画面設計/画面遷移図_A1_プロジェクト管理システム.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9CB6BC-6CD0-4581-BF63-433F501198C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6EC861-76D6-4ED2-949C-A0FBDBFCE7B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4285,6 +4285,73 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>36629</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>51287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>7321</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="正方形/長方形 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAB19AE5-24FD-4EC1-A61E-18F67A6667BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5048244" y="3751383"/>
+          <a:ext cx="249115" cy="344366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+        <a:extLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18000" tIns="7200" rIns="18000" bIns="7200" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -7740,8 +7807,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>105834</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142479</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>80755</xdr:rowOff>
     </xdr:from>
@@ -7764,10 +7831,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="382059" y="3986005"/>
-          <a:ext cx="8592608" cy="2743200"/>
-          <a:chOff x="380378" y="4042034"/>
-          <a:chExt cx="8540501" cy="2796428"/>
+          <a:off x="694929" y="3986005"/>
+          <a:ext cx="8279738" cy="2743200"/>
+          <a:chOff x="691066" y="4042034"/>
+          <a:chExt cx="8229813" cy="2796428"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -7783,10 +7850,10 @@
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="392206" y="5130924"/>
-            <a:ext cx="8528673" cy="1707538"/>
-            <a:chOff x="409680" y="836083"/>
-            <a:chExt cx="8548053" cy="1734931"/>
+            <a:off x="717364" y="5130924"/>
+            <a:ext cx="8203515" cy="1707538"/>
+            <a:chOff x="735564" y="836083"/>
+            <a:chExt cx="8222169" cy="1734931"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -7851,10 +7918,10 @@
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="409680" y="836083"/>
-              <a:ext cx="7996063" cy="1322670"/>
-              <a:chOff x="409680" y="836083"/>
-              <a:chExt cx="7996063" cy="1322670"/>
+              <a:off x="735564" y="836083"/>
+              <a:ext cx="7670179" cy="1322670"/>
+              <a:chOff x="735564" y="836083"/>
+              <a:chExt cx="7670179" cy="1322670"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
@@ -8276,13 +8343,12 @@
               </xdr:cNvPr>
               <xdr:cNvCxnSpPr>
                 <a:cxnSpLocks noChangeShapeType="1"/>
-                <a:endCxn id="60" idx="1"/>
               </xdr:cNvCxnSpPr>
             </xdr:nvCxnSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="409680" y="1739164"/>
-                <a:ext cx="1604282" cy="1"/>
+                <a:off x="735564" y="1739164"/>
+                <a:ext cx="1245331" cy="1"/>
               </a:xfrm>
               <a:prstGeom prst="straightConnector1">
                 <a:avLst/>
@@ -8701,34 +8767,6 @@
                   <a:defRPr sz="1000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                    <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-                    <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:rPr>
-                  <a:t>更新</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="ja-JP" altLang="ja-JP" sz="900" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                    <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-                    <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:rPr>
-                  <a:t>失敗</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-                    <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-                  </a:rPr>
-                  <a:t>/</a:t>
-                </a:r>
-                <a:r>
                   <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
@@ -8754,12 +8792,11 @@
           </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:cxnSpLocks/>
-            <a:stCxn id="51" idx="2"/>
           </xdr:cNvCxnSpPr>
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm rot="5400000">
-            <a:off x="2340877" y="2081535"/>
+            <a:off x="2651565" y="2081535"/>
             <a:ext cx="899136" cy="4820133"/>
           </a:xfrm>
           <a:prstGeom prst="bentConnector2">
@@ -8804,7 +8841,7 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
           <a:xfrm>
-            <a:off x="386890" y="4938825"/>
+            <a:off x="697577" y="4938825"/>
             <a:ext cx="0" cy="1084337"/>
           </a:xfrm>
           <a:prstGeom prst="line">
@@ -8985,6 +9022,253 @@
               <a:ea typeface="ＭＳ 明朝"/>
             </a:rPr>
             <a:t>更新</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="ＭＳ 明朝"/>
+            <a:ea typeface="ＭＳ 明朝"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>124558</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>161187</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>29309</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="直線コネクタ 105">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F767F88-0A64-46D5-B395-B3B4F5DC9770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="32" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="2458180" y="2040551"/>
+          <a:ext cx="659424" cy="4769821"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127815</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>29467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>80457</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>29468</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="AutoShape 294">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CF23349-D588-4FC8-AF79-59921D525E75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks noChangeShapeType="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="406238" y="6220717"/>
+          <a:ext cx="1623181" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>135151</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>22140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>135151</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>32755</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="直線コネクタ 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{463235E1-2FE4-4EB9-B697-8D58914D0DA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="413574" y="4748005"/>
+          <a:ext cx="0" cy="1476000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>262907</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>63792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>134039</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>145699</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="Text Box 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F47F74F-8845-4266-BA27-DC481E82A426}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="819753" y="6255042"/>
+          <a:ext cx="706401" cy="228445"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1100"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="ＭＳ 明朝"/>
+              <a:ea typeface="ＭＳ 明朝"/>
+            </a:rPr>
+            <a:t>戻る</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" altLang="ja-JP" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -16380,7 +16664,7 @@
   <dimension ref="A1:AX33"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AQ48" sqref="AQ48"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -17534,23 +17818,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:N1"/>
+    <mergeCell ref="O1:R3"/>
+    <mergeCell ref="S1:Z3"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:N2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AF2"/>
     <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:N1"/>
-    <mergeCell ref="O1:R3"/>
-    <mergeCell ref="S1:Z3"/>
-    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="AG1:AI1"/>
     <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:N3"/>
   </mergeCells>
   <phoneticPr fontId="8"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>